<commit_message>
add logo image, save img as png format
</commit_message>
<xml_diff>
--- a/paper/04_CRC/LOSO_results_ROC.xlsx
+++ b/paper/04_CRC/LOSO_results_ROC.xlsx
@@ -374,27 +374,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>CHN</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>FRA</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>USA</t>
         </is>
       </c>
     </row>

</xml_diff>